<commit_message>
add proj1 scalability 2
</commit_message>
<xml_diff>
--- a/proj1_centralized_multiuser_bank/doc/records.xlsx
+++ b/proj1_centralized_multiuser_bank/doc/records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/TA/21F_621OS_Nilanjan_Banerjee/git/DistributedOS/proj1_centralized_multiuser_bank/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021773E4-5EF4-704A-AA5B-CB8A4E8D5D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEC4D96-29AD-A54C-9AA2-BDD1C013D3C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -191,17 +191,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Clients amount</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -310,36 +299,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$K$3</c:f>
+              <c:f>Sheet1!$C$4:$K$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>5.9999999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8.5999999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>9.1E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>7.3999999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>7.3499999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>6.4000000000000005E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50</c:v>
+                  <c:v>7.4399999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>75</c:v>
+                  <c:v>1.7424700000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>100</c:v>
+                  <c:v>2.7789999999999998E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -348,169 +337,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-85B8-5740-96F2-D501C5A49EDD}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Transaction avg complete time (ms)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$3:$K$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$4:$K$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>5.9999999999999995E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.5999999999999998E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.1E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.3999999999999999E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.3499999999999998E-4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.4000000000000005E-4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.4399999999999998E-4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.7424700000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.7789999999999998E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-85B8-5740-96F2-D501C5A49EDD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -818,7 +644,673 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Transaction avg complete time (ms) over  </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>transaction rate (one transaction every rate milliseconds)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" b="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$25:$I$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$26:$I$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.8800000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.372E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1919999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.9199999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.9999999999999995E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4040000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.3199999999999999E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3C08-8D43-8801-C07CD9868F91}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:smooth val="0"/>
+        <c:axId val="1434987135"/>
+        <c:axId val="1435377823"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1434987135"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>transaction</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> rate</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1435377823"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1435377823"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Avg time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1434987135"/>
+        <c:crossesAt val="1"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1374,20 +1866,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>325005</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>173183</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>654050</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>519546</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>14433</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1407,6 +2415,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0AEDACE-B264-3D4E-83C0-108C497A9E45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1739,8 +2785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26:F26"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1813,32 +2859,56 @@
         <v>2.7789999999999998E-3</v>
       </c>
     </row>
-    <row r="25" spans="2:7">
+    <row r="25" spans="2:9">
       <c r="B25" t="s">
         <v>2</v>
       </c>
       <c r="C25">
+        <v>0.1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>10</v>
+      </c>
+      <c r="G25">
+        <v>50</v>
+      </c>
+      <c r="H25">
         <v>100</v>
       </c>
-      <c r="D25">
-        <v>250</v>
-      </c>
-      <c r="E25">
-        <v>500</v>
-      </c>
-      <c r="F25">
-        <v>750</v>
-      </c>
-      <c r="G25">
-        <v>1000</v>
+      <c r="I25">
+        <v>200</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="16">
+    <row r="26" spans="2:9" ht="16">
       <c r="B26" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="1">
+        <v>3.8800000000000002E-3</v>
+      </c>
+      <c r="D26">
+        <v>3.372E-3</v>
+      </c>
+      <c r="E26">
+        <v>1.1919999999999999E-3</v>
+      </c>
+      <c r="F26">
+        <v>5.9199999999999997E-4</v>
+      </c>
+      <c r="G26">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="H26" s="1">
         <v>1.4040000000000001E-3</v>
+      </c>
+      <c r="I26">
+        <v>9.3199999999999999E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>